<commit_message>
Update CDM-1 and Add CDM-2
Adicionado CDM-2, resultado da atividade realizada no dia 17/10/2016 e
atualizado o CDM-1 conforme correção prevista pelo CDM-2.
</commit_message>
<xml_diff>
--- a/Projeto/GPR/PG2016-1-CDM-1.xlsx
+++ b/Projeto/GPR/PG2016-1-CDM-1.xlsx
@@ -299,6 +299,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -335,12 +359,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -352,24 +370,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -695,7 +695,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:I4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -708,75 +708,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="15">
+      <c r="B3" s="14"/>
+      <c r="C3" s="23">
         <v>42653</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:11" ht="18">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:11" ht="42.75">
       <c r="A6" s="2" t="s">
@@ -788,14 +788,14 @@
       <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21" t="s">
+      <c r="E6" s="27"/>
+      <c r="F6" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="21"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="2" t="s">
         <v>4</v>
       </c>
@@ -813,20 +813,20 @@
       <c r="C7" s="4">
         <v>6</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="7">
         <v>300</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="25">
+      <c r="E7" s="8"/>
+      <c r="F7" s="7">
         <v>300</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="5">
-        <f>((B7/C7)-1)*100</f>
+        <f>((C7)/B7)-1</f>
         <v>0</v>
       </c>
       <c r="I7" s="5">
-        <f>((D7/F7)-1)*100</f>
+        <f>((F7)/D7)-1</f>
         <v>0</v>
       </c>
     </row>
@@ -840,34 +840,34 @@
       <c r="C8" s="4">
         <v>40</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="7">
         <v>1800</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="25">
+      <c r="E8" s="8"/>
+      <c r="F8" s="7">
         <v>1800</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="8"/>
       <c r="H8" s="5">
-        <f>((B8/C8)-1)*100</f>
+        <f>((C8)/B8)-1</f>
         <v>0</v>
       </c>
       <c r="I8" s="5">
-        <f>((D8/F8)-1)*100</f>
+        <f>((F8)/D8)-1</f>
         <v>0</v>
       </c>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
       <c r="H9" s="5">
         <f>SUM(H7:H8)</f>
         <v>0</v>
@@ -878,15 +878,15 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="5">
         <f>AVERAGE(H7:H8)</f>
         <v>0</v>
@@ -897,127 +897,118 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:11" ht="18">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:11" s="1" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18" t="s">
+      <c r="E15" s="26"/>
+      <c r="F15" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="7"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="8"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="16"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="F16:I16"/>
     <mergeCell ref="A17:I19"/>
@@ -1034,6 +1025,15 @@
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A10:G10"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>